<commit_message>
add more hours for calculus
</commit_message>
<xml_diff>
--- a/serversNamesWillBeChanged.xlsx
+++ b/serversNamesWillBeChanged.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mustafaalogaidi/Desktop/starter-web/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76E2F3B7-BE62-0D47-BCF3-3D0839ACF447}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFB50F22-770B-3D44-A18D-B69D8FD7D0B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" activeTab="4" xr2:uid="{08EF0D23-01A8-4541-9257-D473107B6C11}"/>
   </bookViews>
@@ -2708,7 +2708,7 @@
   <dimension ref="A1:P18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2898,7 +2898,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="36">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I5" s="33">
         <v>0</v>
@@ -3056,7 +3056,7 @@
       </c>
       <c r="H9" s="62">
         <f t="shared" si="0"/>
-        <v>2.5</v>
+        <v>4.5</v>
       </c>
       <c r="I9" s="62">
         <f t="shared" si="0"/>
@@ -3142,7 +3142,7 @@
       </c>
       <c r="H11" s="39">
         <f t="shared" si="1"/>
-        <v>4.5</v>
+        <v>2.5</v>
       </c>
       <c r="I11" s="39">
         <f t="shared" si="1"/>
@@ -3205,7 +3205,7 @@
       </c>
       <c r="B13" s="45">
         <f>SUM(C11:L11)</f>
-        <v>23.5</v>
+        <v>21.5</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
update with math hours
</commit_message>
<xml_diff>
--- a/serversNamesWillBeChanged.xlsx
+++ b/serversNamesWillBeChanged.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mustafaalogaidi/Desktop/starter-web/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DF3F390-FDEE-A44B-BFE7-29A775DB5A9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1A74DB6-CFF4-6445-88C5-97E44B5A050A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" activeTab="4" xr2:uid="{08EF0D23-01A8-4541-9257-D473107B6C11}"/>
   </bookViews>
@@ -2709,7 +2709,7 @@
   <dimension ref="A1:P18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2928,7 +2928,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" s="33">
         <v>0</v>
@@ -3045,7 +3045,7 @@
       </c>
       <c r="E9" s="62">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F9" s="62">
         <f t="shared" si="0"/>
@@ -3131,7 +3131,7 @@
       </c>
       <c r="E11" s="39">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11" s="39">
         <f t="shared" si="1"/>
@@ -3206,7 +3206,7 @@
       </c>
       <c r="B13" s="45">
         <f>SUM(C11:L11)</f>
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
remove AI this week,
</commit_message>
<xml_diff>
--- a/serversNamesWillBeChanged.xlsx
+++ b/serversNamesWillBeChanged.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mustafaalogaidi/Desktop/starter-web/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1A74DB6-CFF4-6445-88C5-97E44B5A050A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFF8DD33-5C7A-9049-A9E9-CAB347BD0044}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" activeTab="4" xr2:uid="{08EF0D23-01A8-4541-9257-D473107B6C11}"/>
   </bookViews>
@@ -2709,7 +2709,7 @@
   <dimension ref="A1:P18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3084,7 +3084,7 @@
         <v>159</v>
       </c>
       <c r="C10" s="59">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D10" s="59">
         <v>10</v>
@@ -3123,7 +3123,7 @@
       </c>
       <c r="C11" s="39">
         <f>C10-C9</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D11" s="39">
         <f t="shared" ref="D11:L11" si="1">D10-D9</f>
@@ -3170,7 +3170,7 @@
         <v>159</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>86</v>
+        <v>165</v>
       </c>
       <c r="D12" s="29" t="s">
         <v>86</v>
@@ -3206,7 +3206,7 @@
       </c>
       <c r="B13" s="45">
         <f>SUM(C11:L11)</f>
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
start new week 12/2
</commit_message>
<xml_diff>
--- a/serversNamesWillBeChanged.xlsx
+++ b/serversNamesWillBeChanged.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mustafaalogaidi/Desktop/starter-web/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v435431\Desktop\DevOps\starter-web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{349739A8-7624-3540-97D2-38D3DF748F3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1572F3EB-B8E2-4476-A46D-D72B257C1F17}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" activeTab="4" xr2:uid="{08EF0D23-01A8-4541-9257-D473107B6C11}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{08EF0D23-01A8-4541-9257-D473107B6C11}"/>
   </bookViews>
   <sheets>
     <sheet name="abc and npd" sheetId="1" r:id="rId1"/>
@@ -728,7 +728,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -789,17 +789,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -825,7 +814,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -936,23 +925,20 @@
     <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="11" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="13" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="13" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -964,13 +950,13 @@
     <xf numFmtId="166" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="14" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="14" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="14" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="6" fillId="14" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1582,14 +1568,14 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.6640625" customWidth="1"/>
-    <col min="3" max="3" width="39.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.7109375" customWidth="1"/>
+    <col min="3" max="3" width="39.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>36</v>
       </c>
@@ -1600,12 +1586,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -1616,7 +1602,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -1627,7 +1613,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
@@ -1638,7 +1624,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -1649,7 +1635,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -1660,7 +1646,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>3</v>
       </c>
@@ -1671,12 +1657,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>7</v>
       </c>
@@ -1687,7 +1673,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
@@ -1698,7 +1684,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>6</v>
       </c>
@@ -1709,7 +1695,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>10</v>
       </c>
@@ -1720,7 +1706,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>11</v>
       </c>
@@ -1731,7 +1717,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>9</v>
       </c>
@@ -1742,59 +1728,59 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>20</v>
       </c>
@@ -1805,7 +1791,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>21</v>
       </c>
@@ -1816,7 +1802,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>19</v>
       </c>
@@ -1827,7 +1813,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>23</v>
       </c>
@@ -1838,7 +1824,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>18</v>
       </c>
@@ -1849,7 +1835,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>22</v>
       </c>
@@ -1860,12 +1846,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>28</v>
       </c>
@@ -1876,7 +1862,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>29</v>
       </c>
@@ -1887,7 +1873,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>27</v>
       </c>
@@ -1898,7 +1884,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>24</v>
       </c>
@@ -1909,7 +1895,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>25</v>
       </c>
@@ -1920,7 +1906,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>26</v>
       </c>
@@ -1931,12 +1917,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>35</v>
       </c>
@@ -1947,7 +1933,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>34</v>
       </c>
@@ -1958,7 +1944,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>30</v>
       </c>
@@ -1969,7 +1955,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>33</v>
       </c>
@@ -1980,7 +1966,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>32</v>
       </c>
@@ -1991,7 +1977,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>31</v>
       </c>
@@ -2002,12 +1988,12 @@
         <v>68</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
       <c r="B45" s="3" t="s">
         <v>57</v>
@@ -2016,7 +2002,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
       <c r="B46" s="3" t="s">
         <v>58</v>
@@ -2025,7 +2011,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
       <c r="B47" s="3" t="s">
         <v>59</v>
@@ -2034,7 +2020,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
       <c r="B48" s="3" t="s">
         <v>60</v>
@@ -2043,7 +2029,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
       <c r="B49" s="3" t="s">
         <v>61</v>
@@ -2052,7 +2038,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
       <c r="B50" s="3" t="s">
         <v>62</v>
@@ -2061,12 +2047,12 @@
         <v>62</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>152</v>
       </c>
@@ -2077,7 +2063,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>153</v>
       </c>
@@ -2088,7 +2074,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>154</v>
       </c>
@@ -2099,7 +2085,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>155</v>
       </c>
@@ -2110,7 +2096,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>156</v>
       </c>
@@ -2121,7 +2107,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>157</v>
       </c>
@@ -2176,202 +2162,202 @@
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="16"/>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="16"/>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="16"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="16"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="16"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>123</v>
       </c>
@@ -2390,13 +2376,13 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="45.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="45.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>126</v>
       </c>
@@ -2407,12 +2393,12 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
         <v>134</v>
       </c>
@@ -2421,7 +2407,7 @@
       </c>
       <c r="C3" s="28"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
         <v>135</v>
       </c>
@@ -2430,7 +2416,7 @@
       </c>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
         <v>136</v>
       </c>
@@ -2439,7 +2425,7 @@
       </c>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>137</v>
       </c>
@@ -2448,12 +2434,12 @@
       </c>
       <c r="C6" s="28"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="16"/>
       <c r="B7" s="16"/>
       <c r="C7" s="3"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
         <v>124</v>
       </c>
@@ -2462,7 +2448,7 @@
       </c>
       <c r="C8" s="28"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
         <v>128</v>
       </c>
@@ -2471,7 +2457,7 @@
       </c>
       <c r="C9" s="3"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
         <v>130</v>
       </c>
@@ -2480,7 +2466,7 @@
       </c>
       <c r="C10" s="3"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
         <v>131</v>
       </c>
@@ -2489,12 +2475,12 @@
       </c>
       <c r="C11" s="3"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="16"/>
       <c r="B12" s="16"/>
       <c r="C12" s="3"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="25" t="s">
         <v>125</v>
       </c>
@@ -2503,7 +2489,7 @@
       </c>
       <c r="C13" s="28"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
         <v>129</v>
       </c>
@@ -2512,7 +2498,7 @@
       </c>
       <c r="C14" s="3"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="25" t="s">
         <v>132</v>
       </c>
@@ -2521,7 +2507,7 @@
       </c>
       <c r="C15" s="3"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
         <v>133</v>
       </c>
@@ -2530,7 +2516,7 @@
       </c>
       <c r="C16" s="3"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="19"/>
     </row>
   </sheetData>
@@ -2558,13 +2544,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>138</v>
       </c>
@@ -2572,11 +2558,11 @@
         <v>139</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="22"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>141</v>
       </c>
@@ -2584,7 +2570,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>140</v>
       </c>
@@ -2592,7 +2578,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>142</v>
       </c>
@@ -2600,7 +2586,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
         <v>143</v>
       </c>
@@ -2608,7 +2594,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
         <v>144</v>
       </c>
@@ -2616,7 +2602,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
         <v>145</v>
       </c>
@@ -2624,7 +2610,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
         <v>146</v>
       </c>
@@ -2632,7 +2618,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
         <v>147</v>
       </c>
@@ -2640,7 +2626,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
         <v>148</v>
       </c>
@@ -2648,7 +2634,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
         <v>149</v>
       </c>
@@ -2656,7 +2642,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
         <v>150</v>
       </c>
@@ -2664,7 +2650,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>151</v>
       </c>
@@ -2672,7 +2658,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B16" s="24"/>
     </row>
   </sheetData>
@@ -2708,29 +2694,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3746CAEE-2743-4F46-B291-636CFD381F54}">
   <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5" customWidth="1"/>
-    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" customWidth="1"/>
-    <col min="11" max="11" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.33203125" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="14"/>
       <c r="B1" s="14"/>
-      <c r="C1" s="63" t="s">
+      <c r="C1" s="62" t="s">
         <v>71</v>
       </c>
       <c r="D1" s="6" t="s">
@@ -2762,21 +2748,21 @@
       </c>
       <c r="P1" s="42"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="31">
-        <v>43794</v>
+        <v>43801</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="C2" s="64">
+      <c r="C2" s="63">
         <v>0</v>
       </c>
       <c r="D2" s="33">
         <v>0</v>
       </c>
       <c r="E2" s="34">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F2" s="33">
         <v>0</v>
@@ -2800,21 +2786,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="31">
-        <v>43795</v>
+        <v>43802</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C3" s="64">
+      <c r="C3" s="63">
         <v>0</v>
       </c>
       <c r="D3" s="33">
         <v>0</v>
       </c>
       <c r="E3" s="34">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="F3" s="48">
         <v>0</v>
@@ -2823,7 +2809,7 @@
         <v>0</v>
       </c>
       <c r="H3" s="36">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="I3" s="33">
         <v>0</v>
@@ -2838,14 +2824,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="31">
-        <v>43796</v>
+        <v>43803</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C4" s="64">
+      <c r="C4" s="63">
         <v>0</v>
       </c>
       <c r="D4" s="33">
@@ -2861,7 +2847,7 @@
         <v>0</v>
       </c>
       <c r="H4" s="36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4" s="33">
         <v>0</v>
@@ -2876,21 +2862,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="31">
-        <v>43797</v>
+        <v>43804</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C5" s="64">
+      <c r="C5" s="63">
         <v>0</v>
       </c>
       <c r="D5" s="33">
         <v>0</v>
       </c>
       <c r="E5" s="34">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F5" s="48">
         <v>0</v>
@@ -2899,7 +2885,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="36">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I5" s="33">
         <v>0</v>
@@ -2914,9 +2900,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="31">
-        <v>43798</v>
+        <v>43805</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>81</v>
@@ -2928,7 +2914,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" s="33">
         <v>0</v>
@@ -2937,7 +2923,7 @@
         <v>0</v>
       </c>
       <c r="H6" s="36">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="I6" s="33">
         <v>0</v>
@@ -2952,9 +2938,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="31">
-        <v>43799</v>
+        <v>43806</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>82</v>
@@ -2963,158 +2949,158 @@
         <v>0</v>
       </c>
       <c r="D7" s="37">
+        <v>0</v>
+      </c>
+      <c r="E7" s="38">
+        <v>0</v>
+      </c>
+      <c r="F7" s="48">
+        <v>0</v>
+      </c>
+      <c r="G7" s="47">
+        <v>0</v>
+      </c>
+      <c r="H7" s="46">
+        <v>0</v>
+      </c>
+      <c r="I7" s="33">
+        <v>0</v>
+      </c>
+      <c r="J7" s="33">
+        <v>0</v>
+      </c>
+      <c r="K7" s="33">
+        <v>0</v>
+      </c>
+      <c r="L7" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="31">
+        <v>43807</v>
+      </c>
+      <c r="B8" s="50" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" s="51">
+        <v>0</v>
+      </c>
+      <c r="D8" s="52">
+        <v>0</v>
+      </c>
+      <c r="E8" s="53">
+        <v>0</v>
+      </c>
+      <c r="F8" s="51">
+        <v>0</v>
+      </c>
+      <c r="G8" s="54">
+        <v>0</v>
+      </c>
+      <c r="H8" s="55">
+        <v>0</v>
+      </c>
+      <c r="I8" s="51">
+        <v>0</v>
+      </c>
+      <c r="J8" s="51">
+        <v>0</v>
+      </c>
+      <c r="K8" s="51">
+        <v>0</v>
+      </c>
+      <c r="L8" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="B9" s="60" t="s">
+        <v>159</v>
+      </c>
+      <c r="C9" s="61">
+        <f>SUM(C2:C8)</f>
+        <v>0</v>
+      </c>
+      <c r="D9" s="61">
+        <f t="shared" ref="D9:L9" si="0">SUM(D2:D8)</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="61">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F9" s="61">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G9" s="61">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H9" s="61">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I9" s="61">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J9" s="61">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K9" s="61">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L9" s="61">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="56" t="s">
+        <v>162</v>
+      </c>
+      <c r="B10" s="57" t="s">
+        <v>159</v>
+      </c>
+      <c r="C10" s="58">
+        <v>2</v>
+      </c>
+      <c r="D10" s="58">
+        <v>10</v>
+      </c>
+      <c r="E10" s="58">
         <v>5</v>
       </c>
-      <c r="E7" s="38">
-        <v>0</v>
-      </c>
-      <c r="F7" s="48">
-        <v>1</v>
-      </c>
-      <c r="G7" s="47">
-        <v>0</v>
-      </c>
-      <c r="H7" s="46">
-        <v>0</v>
-      </c>
-      <c r="I7" s="33">
-        <v>0</v>
-      </c>
-      <c r="J7" s="33">
-        <v>0</v>
-      </c>
-      <c r="K7" s="33">
-        <v>0</v>
-      </c>
-      <c r="L7" s="33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A8" s="50">
-        <v>43800</v>
-      </c>
-      <c r="B8" s="51" t="s">
-        <v>83</v>
-      </c>
-      <c r="C8" s="52">
-        <v>0</v>
-      </c>
-      <c r="D8" s="53">
-        <v>3</v>
-      </c>
-      <c r="E8" s="54">
-        <v>0</v>
-      </c>
-      <c r="F8" s="52">
-        <v>1</v>
-      </c>
-      <c r="G8" s="55">
-        <v>0</v>
-      </c>
-      <c r="H8" s="56">
-        <v>0</v>
-      </c>
-      <c r="I8" s="52">
-        <v>0</v>
-      </c>
-      <c r="J8" s="52">
-        <v>0</v>
-      </c>
-      <c r="K8" s="52">
-        <v>0</v>
-      </c>
-      <c r="L8" s="52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A9" s="60" t="s">
-        <v>158</v>
-      </c>
-      <c r="B9" s="61" t="s">
-        <v>159</v>
-      </c>
-      <c r="C9" s="62">
-        <f>SUM(C2:C8)</f>
-        <v>0</v>
-      </c>
-      <c r="D9" s="62">
-        <f t="shared" ref="D9:L9" si="0">SUM(D2:D8)</f>
-        <v>8</v>
-      </c>
-      <c r="E9" s="62">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="F9" s="62">
-        <f t="shared" si="0"/>
+      <c r="F10" s="58">
         <v>2</v>
       </c>
-      <c r="G9" s="62">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H9" s="62">
-        <f t="shared" si="0"/>
+      <c r="G10" s="58">
+        <v>2</v>
+      </c>
+      <c r="H10" s="58">
         <v>7</v>
       </c>
-      <c r="I9" s="62">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J9" s="62">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K9" s="62">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L9" s="62">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A10" s="57" t="s">
-        <v>162</v>
-      </c>
-      <c r="B10" s="58" t="s">
-        <v>159</v>
-      </c>
-      <c r="C10" s="59">
-        <v>2</v>
-      </c>
-      <c r="D10" s="59">
-        <v>10</v>
-      </c>
-      <c r="E10" s="59">
-        <v>5</v>
-      </c>
-      <c r="F10" s="59">
-        <v>2</v>
-      </c>
-      <c r="G10" s="59">
-        <v>2</v>
-      </c>
-      <c r="H10" s="59">
-        <v>7</v>
-      </c>
-      <c r="I10" s="59">
-        <v>0</v>
-      </c>
-      <c r="J10" s="59">
-        <v>0</v>
-      </c>
-      <c r="K10" s="59">
-        <v>0</v>
-      </c>
-      <c r="L10" s="59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="I10" s="58">
+        <v>0</v>
+      </c>
+      <c r="J10" s="58">
+        <v>0</v>
+      </c>
+      <c r="K10" s="58">
+        <v>0</v>
+      </c>
+      <c r="L10" s="58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="49" t="s">
         <v>163</v>
       </c>
@@ -3127,15 +3113,15 @@
       </c>
       <c r="D11" s="39">
         <f t="shared" ref="D11:L11" si="1">D10-D9</f>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E11" s="39">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F11" s="39">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G11" s="39">
         <f t="shared" si="1"/>
@@ -3143,7 +3129,7 @@
       </c>
       <c r="H11" s="39">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I11" s="39">
         <f t="shared" si="1"/>
@@ -3162,7 +3148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>85</v>
       </c>
@@ -3200,30 +3186,30 @@
         <v>165</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="44" t="s">
         <v>166</v>
       </c>
       <c r="B13" s="45">
         <f>SUM(C11:L11)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A15" s="65" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="64" t="s">
         <v>167</v>
       </c>
       <c r="C15" s="40"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A16" s="66" t="s">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="65" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="17" spans="4:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D17" s="32"/>
     </row>
-    <row r="18" spans="4:16" ht="32" x14ac:dyDescent="0.2">
+    <row r="18" spans="4:16" ht="30" x14ac:dyDescent="0.25">
       <c r="P18" s="43" t="s">
         <v>164</v>
       </c>

</xml_diff>

<commit_message>
add blockchain and AI hours for this week
</commit_message>
<xml_diff>
--- a/serversNamesWillBeChanged.xlsx
+++ b/serversNamesWillBeChanged.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v435431\Desktop\DevOps\starter-web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08A6F1D9-9485-4303-A1AD-C10A45F65387}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E6C88C3-81E4-4321-B246-28CBA201D4BD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{08EF0D23-01A8-4541-9257-D473107B6C11}"/>
   </bookViews>
@@ -2695,7 +2695,7 @@
   <dimension ref="A1:P18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A8"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2756,7 +2756,7 @@
         <v>77</v>
       </c>
       <c r="C2" s="63">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D2" s="33">
         <v>0</v>
@@ -2768,7 +2768,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="35">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H2" s="36">
         <v>0</v>
@@ -3023,7 +3023,7 @@
       </c>
       <c r="C9" s="61">
         <f>SUM(C2:C8)</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D9" s="61">
         <f t="shared" ref="D9:L9" si="0">SUM(D2:D8)</f>
@@ -3039,7 +3039,7 @@
       </c>
       <c r="G9" s="61">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H9" s="61">
         <f t="shared" si="0"/>
@@ -3109,7 +3109,7 @@
       </c>
       <c r="C11" s="39">
         <f>C10-C9</f>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="D11" s="39">
         <f t="shared" ref="D11:L11" si="1">D10-D9</f>
@@ -3125,7 +3125,7 @@
       </c>
       <c r="G11" s="39">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="H11" s="39">
         <f t="shared" si="1"/>
@@ -3192,7 +3192,7 @@
       </c>
       <c r="B13" s="45">
         <f>SUM(C11:L11)</f>
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update hours for monday
</commit_message>
<xml_diff>
--- a/serversNamesWillBeChanged.xlsx
+++ b/serversNamesWillBeChanged.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v435431\Desktop\DevOps\starter-web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E6C88C3-81E4-4321-B246-28CBA201D4BD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13EF9617-11F0-420D-A3A2-75EE954D7A98}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{08EF0D23-01A8-4541-9257-D473107B6C11}"/>
   </bookViews>
@@ -20,6 +20,7 @@
     <sheet name="Agenda" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2695,7 +2696,7 @@
   <dimension ref="A1:P18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2762,7 +2763,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2" s="33">
         <v>0</v>
@@ -2771,7 +2772,7 @@
         <v>0.5</v>
       </c>
       <c r="H2" s="36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I2" s="33">
         <v>0</v>
@@ -3031,7 +3032,7 @@
       </c>
       <c r="E9" s="61">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9" s="61">
         <f t="shared" si="0"/>
@@ -3043,7 +3044,7 @@
       </c>
       <c r="H9" s="61">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9" s="61">
         <f t="shared" si="0"/>
@@ -3117,7 +3118,7 @@
       </c>
       <c r="E11" s="39">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F11" s="39">
         <f t="shared" si="1"/>
@@ -3129,7 +3130,7 @@
       </c>
       <c r="H11" s="39">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I11" s="39">
         <f t="shared" si="1"/>
@@ -3192,7 +3193,7 @@
       </c>
       <c r="B13" s="45">
         <f>SUM(C11:L11)</f>
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
update Excel Sheet by adding fast reading hours
</commit_message>
<xml_diff>
--- a/serversNamesWillBeChanged.xlsx
+++ b/serversNamesWillBeChanged.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v435431\Desktop\DevOps\starter-web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53FCFE7C-D6C1-4A7F-B9E9-A29CB100514E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B86F39C9-597E-44BA-BC24-75033EE89642}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{08EF0D23-01A8-4541-9257-D473107B6C11}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{08EF0D23-01A8-4541-9257-D473107B6C11}"/>
   </bookViews>
   <sheets>
     <sheet name="abc and npd" sheetId="1" r:id="rId1"/>
@@ -1005,7 +1005,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="130">
+  <dxfs count="47">
     <dxf>
       <fill>
         <patternFill>
@@ -1045,587 +1045,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2792,32 +2211,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:B50">
-    <cfRule type="expression" dxfId="129" priority="9">
+    <cfRule type="expression" dxfId="46" priority="9">
       <formula>AND($B3="",$A3="")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="128" priority="10">
+    <cfRule type="expression" dxfId="45" priority="10">
       <formula>$B3&lt;&gt;$A3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="127" priority="12">
+    <cfRule type="expression" dxfId="44" priority="12">
       <formula>$B3=$A3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C50">
-    <cfRule type="expression" dxfId="126" priority="4">
+    <cfRule type="expression" dxfId="43" priority="4">
       <formula>AND($C3="",$B3="")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="125" priority="5">
+    <cfRule type="expression" dxfId="42" priority="5">
       <formula>$C3&lt;&gt;$B3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="124" priority="7">
+    <cfRule type="expression" dxfId="41" priority="7">
       <formula>AND($C3=$B3,$C3=$A3)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="123" priority="8">
+    <cfRule type="expression" dxfId="40" priority="8">
       <formula>$C3=$B3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:A57">
-    <cfRule type="expression" dxfId="122" priority="1">
+    <cfRule type="expression" dxfId="39" priority="1">
       <formula>$A3=""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3193,13 +2612,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:B16">
-    <cfRule type="expression" dxfId="121" priority="1">
+    <cfRule type="expression" dxfId="38" priority="1">
       <formula>$B3=""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="120" priority="2">
+    <cfRule type="expression" dxfId="37" priority="2">
       <formula>$B3=$A3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="119" priority="3">
+    <cfRule type="expression" dxfId="36" priority="3">
       <formula>$B3&lt;&gt;$A3</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3335,25 +2754,25 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:B14 B14">
-    <cfRule type="expression" dxfId="118" priority="7">
+    <cfRule type="expression" dxfId="35" priority="7">
       <formula>$B3=$A3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:A14">
-    <cfRule type="expression" dxfId="117" priority="2">
+    <cfRule type="expression" dxfId="34" priority="2">
       <formula>$A3=""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="116" priority="3">
+    <cfRule type="expression" dxfId="33" priority="3">
       <formula>$A3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B14">
-    <cfRule type="expression" dxfId="115" priority="4">
+    <cfRule type="expression" dxfId="32" priority="4">
       <formula>$B3=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B14">
-    <cfRule type="expression" dxfId="114" priority="5">
+    <cfRule type="expression" dxfId="31" priority="5">
       <formula>$B3&lt;&gt;$A3</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3364,10 +2783,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3746CAEE-2743-4F46-B291-636CFD381F54}">
-  <dimension ref="A1:P18"/>
+  <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3862,22 +3281,22 @@
         <v>159</v>
       </c>
       <c r="C10" s="61">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D10" s="61">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E10" s="61">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F10" s="61">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G10" s="61">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H10" s="61">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="I10" s="61">
         <v>0</v>
@@ -3901,7 +3320,7 @@
         <v>0</v>
       </c>
       <c r="P10" s="68">
-        <v>3.5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -3913,27 +3332,27 @@
       </c>
       <c r="C11" s="62">
         <f>C10-C9</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D11" s="62">
         <f t="shared" ref="D11:L11" si="2">D10-D9</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E11" s="62">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F11" s="62">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G11" s="62">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H11" s="62">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="I11" s="62">
         <f t="shared" si="2"/>
@@ -3965,7 +3384,7 @@
       </c>
       <c r="P11" s="62">
         <f>P10-P9</f>
-        <v>3.5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -4024,7 +3443,7 @@
       </c>
       <c r="B13" s="63">
         <f>SUM(C11:L11)</f>
-        <v>32</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
@@ -4038,139 +3457,159 @@
         <v>168</v>
       </c>
     </row>
-    <row r="17" spans="4:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:16" x14ac:dyDescent="0.25">
       <c r="D17" s="32"/>
     </row>
-    <row r="18" spans="4:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:16" ht="30" x14ac:dyDescent="0.25">
       <c r="P18" s="35" t="s">
         <v>164</v>
       </c>
     </row>
+    <row r="19" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C19" s="61">
+        <v>2</v>
+      </c>
+      <c r="D19" s="61">
+        <v>10</v>
+      </c>
+      <c r="E19" s="61">
+        <v>5</v>
+      </c>
+      <c r="F19" s="61">
+        <v>4</v>
+      </c>
+      <c r="G19" s="61">
+        <v>4</v>
+      </c>
+      <c r="H19" s="61">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="C11">
-    <cfRule type="expression" dxfId="61" priority="32">
+    <cfRule type="expression" dxfId="30" priority="32">
       <formula>$C11=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="35">
+    <cfRule type="expression" dxfId="29" priority="35">
       <formula>$C11&lt;&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11">
-    <cfRule type="expression" dxfId="59" priority="31">
+    <cfRule type="expression" dxfId="28" priority="31">
       <formula>$D11=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="30">
+    <cfRule type="expression" dxfId="27" priority="30">
       <formula>$D11&lt;&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="expression" dxfId="57" priority="28">
+    <cfRule type="expression" dxfId="26" priority="28">
       <formula>$E11=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="27">
+    <cfRule type="expression" dxfId="25" priority="27">
       <formula>$E11&lt;&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F11">
-    <cfRule type="expression" dxfId="55" priority="26">
+    <cfRule type="expression" dxfId="24" priority="26">
       <formula>$F11=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="25">
+    <cfRule type="expression" dxfId="23" priority="25">
       <formula>$F11&lt;&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G11">
-    <cfRule type="expression" dxfId="53" priority="24">
+    <cfRule type="expression" dxfId="22" priority="24">
       <formula>$G11=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="23">
+    <cfRule type="expression" dxfId="21" priority="23">
       <formula>$G11&lt;&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11">
-    <cfRule type="expression" dxfId="51" priority="21">
+    <cfRule type="expression" dxfId="20" priority="21">
       <formula>$H11&lt;&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="22">
+    <cfRule type="expression" dxfId="19" priority="22">
       <formula>$H11=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I11">
-    <cfRule type="expression" dxfId="49" priority="19">
+    <cfRule type="expression" dxfId="18" priority="19">
       <formula>$I11&lt;&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="20">
+    <cfRule type="expression" dxfId="17" priority="20">
       <formula>$I11=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11">
-    <cfRule type="expression" dxfId="47" priority="17">
+    <cfRule type="expression" dxfId="16" priority="17">
       <formula>$J11&lt;&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="18">
+    <cfRule type="expression" dxfId="15" priority="18">
       <formula>$J11=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11">
-    <cfRule type="expression" dxfId="45" priority="15">
+    <cfRule type="expression" dxfId="14" priority="15">
       <formula>$K11&lt;&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="16">
+    <cfRule type="expression" dxfId="13" priority="16">
       <formula>$K11=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L11">
-    <cfRule type="expression" dxfId="43" priority="13">
+    <cfRule type="expression" dxfId="12" priority="13">
       <formula>$L11&lt;&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="14">
+    <cfRule type="expression" dxfId="11" priority="14">
       <formula>$L11=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11">
-    <cfRule type="expression" dxfId="41" priority="12">
+    <cfRule type="expression" dxfId="10" priority="12">
       <formula>OR($C11&lt;&gt;0,$D11&lt;&gt;0,$E11&lt;&gt;0,$F11&lt;&gt;0,$G11&lt;&gt;0,$H11&lt;&gt;0,$I11&lt;&gt;0,$J11&lt;&gt;0,$K11&lt;&gt;0,$L11&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="expression" dxfId="40" priority="11">
+    <cfRule type="expression" dxfId="9" priority="11">
       <formula>OR($C11&lt;&gt;0,$D11&lt;&gt;0,$E11&lt;&gt;0,$F11&lt;&gt;0,$G11&lt;&gt;0,$H11&lt;&gt;0,$I11&lt;&gt;0,$J11&lt;&gt;0,$K11&lt;&gt;0,$L11&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="expression" dxfId="39" priority="9">
+    <cfRule type="expression" dxfId="8" priority="9">
       <formula>$B13&lt;30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N11">
-    <cfRule type="expression" dxfId="38" priority="7">
+    <cfRule type="expression" dxfId="7" priority="7">
       <formula>$N11&lt;&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="8">
+    <cfRule type="expression" dxfId="6" priority="8">
       <formula>$N11=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M11">
-    <cfRule type="expression" dxfId="36" priority="6">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>$M11&lt;&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="5">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>$N11=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O11">
-    <cfRule type="expression" dxfId="34" priority="4">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>$O11&lt;&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>$O11=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P11">
-    <cfRule type="expression" dxfId="32" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>$P11=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="2">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>$P11&lt;&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
focus on fast reading and printing
</commit_message>
<xml_diff>
--- a/serversNamesWillBeChanged.xlsx
+++ b/serversNamesWillBeChanged.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v435431\Desktop\DevOps\starter-web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B86F39C9-597E-44BA-BC24-75033EE89642}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26D0B1A3-4024-4F1C-BDA1-3879F50C2FC1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{08EF0D23-01A8-4541-9257-D473107B6C11}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="174">
   <si>
     <t>Win 2012 ADC PRD</t>
   </si>
@@ -554,7 +554,10 @@
     <t>Terraform for Asure</t>
   </si>
   <si>
-    <t>Fast Reading</t>
+    <t>Fast Reading 500 WPM</t>
+  </si>
+  <si>
+    <t>Fast Typing</t>
   </si>
 </sst>
 </file>
@@ -1005,7 +1008,21 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="47">
+  <dxfs count="49">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2211,32 +2228,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:B50">
-    <cfRule type="expression" dxfId="46" priority="9">
+    <cfRule type="expression" dxfId="48" priority="9">
       <formula>AND($B3="",$A3="")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="10">
+    <cfRule type="expression" dxfId="47" priority="10">
       <formula>$B3&lt;&gt;$A3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="12">
+    <cfRule type="expression" dxfId="46" priority="12">
       <formula>$B3=$A3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C50">
-    <cfRule type="expression" dxfId="43" priority="4">
+    <cfRule type="expression" dxfId="45" priority="4">
       <formula>AND($C3="",$B3="")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="5">
+    <cfRule type="expression" dxfId="44" priority="5">
       <formula>$C3&lt;&gt;$B3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="7">
+    <cfRule type="expression" dxfId="43" priority="7">
       <formula>AND($C3=$B3,$C3=$A3)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="8">
+    <cfRule type="expression" dxfId="42" priority="8">
       <formula>$C3=$B3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:A57">
-    <cfRule type="expression" dxfId="39" priority="1">
+    <cfRule type="expression" dxfId="41" priority="1">
       <formula>$A3=""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2612,13 +2629,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:B16">
-    <cfRule type="expression" dxfId="38" priority="1">
+    <cfRule type="expression" dxfId="40" priority="1">
       <formula>$B3=""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="2">
+    <cfRule type="expression" dxfId="39" priority="2">
       <formula>$B3=$A3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="3">
+    <cfRule type="expression" dxfId="38" priority="3">
       <formula>$B3&lt;&gt;$A3</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2754,25 +2771,25 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:B14 B14">
-    <cfRule type="expression" dxfId="35" priority="7">
+    <cfRule type="expression" dxfId="37" priority="7">
       <formula>$B3=$A3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:A14">
-    <cfRule type="expression" dxfId="34" priority="2">
+    <cfRule type="expression" dxfId="36" priority="2">
       <formula>$A3=""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="3">
+    <cfRule type="expression" dxfId="35" priority="3">
       <formula>$A3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B14">
-    <cfRule type="expression" dxfId="32" priority="4">
+    <cfRule type="expression" dxfId="34" priority="4">
       <formula>$B3=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B14">
-    <cfRule type="expression" dxfId="31" priority="5">
+    <cfRule type="expression" dxfId="33" priority="5">
       <formula>$B3&lt;&gt;$A3</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2783,10 +2800,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3746CAEE-2743-4F46-B291-636CFD381F54}">
-  <dimension ref="A1:P19"/>
+  <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A2" sqref="A2:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2803,10 +2821,11 @@
     <col min="12" max="12" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.28515625" customWidth="1"/>
+    <col min="16" max="16" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="14"/>
       <c r="B1" s="14"/>
       <c r="C1" s="43" t="s">
@@ -2851,10 +2870,13 @@
       <c r="P1" s="67" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q1" s="67" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="31">
-        <v>43808</v>
+        <v>43843</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>77</v>
@@ -2899,13 +2921,15 @@
         <v>0</v>
       </c>
       <c r="P2" s="47">
-        <f t="shared" ref="P2:P9" si="0">SUM(C2:O2)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="31">
-        <v>43809</v>
+        <v>43844</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>78</v>
@@ -2950,13 +2974,15 @@
         <v>0</v>
       </c>
       <c r="P3" s="47">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="31">
-        <v>43810</v>
+        <v>43845</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>79</v>
@@ -3001,13 +3027,15 @@
         <v>0</v>
       </c>
       <c r="P4" s="47">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="31">
-        <v>43811</v>
+        <v>43846</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>80</v>
@@ -3052,13 +3080,15 @@
         <v>0</v>
       </c>
       <c r="P5" s="47">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="31">
-        <v>43812</v>
+        <v>43847</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>81</v>
@@ -3103,13 +3133,16 @@
         <v>0</v>
       </c>
       <c r="P6" s="47">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" ref="P2:P9" si="0">SUM(C6:O6)</f>
+        <v>0</v>
+      </c>
+      <c r="Q6" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="31">
-        <v>43813</v>
+        <v>43848</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>82</v>
@@ -3154,13 +3187,15 @@
         <v>0</v>
       </c>
       <c r="P7" s="47">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="31">
-        <v>43814</v>
+        <v>43849</v>
       </c>
       <c r="B8" s="38" t="s">
         <v>83</v>
@@ -3205,11 +3240,13 @@
         <v>0</v>
       </c>
       <c r="P8" s="47">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="41" t="s">
         <v>158</v>
       </c>
@@ -3269,11 +3306,15 @@
         <v>0</v>
       </c>
       <c r="P9" s="60">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+        <f>SUM(P2:P8)</f>
+        <v>0</v>
+      </c>
+      <c r="Q9" s="60">
+        <f>SUM(Q2:Q8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="39" t="s">
         <v>162</v>
       </c>
@@ -3320,10 +3361,13 @@
         <v>0</v>
       </c>
       <c r="P10" s="68">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="Q10" s="68">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="37" t="s">
         <v>163</v>
       </c>
@@ -3384,10 +3428,14 @@
       </c>
       <c r="P11" s="62">
         <f>P10-P9</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="Q11" s="62">
+        <f>Q10-Q9</f>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>85</v>
       </c>
@@ -3436,8 +3484,11 @@
       <c r="P12" s="29" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q12" s="29" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="36" t="s">
         <v>166</v>
       </c>
@@ -3446,13 +3497,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="44" t="s">
         <v>167</v>
       </c>
       <c r="C15" s="33"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="45" t="s">
         <v>168</v>
       </c>
@@ -3487,125 +3538,133 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C11">
-    <cfRule type="expression" dxfId="30" priority="32">
+    <cfRule type="expression" dxfId="32" priority="34">
       <formula>$C11=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="35">
+    <cfRule type="expression" dxfId="31" priority="37">
       <formula>$C11&lt;&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11">
-    <cfRule type="expression" dxfId="28" priority="31">
+    <cfRule type="expression" dxfId="30" priority="33">
       <formula>$D11=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="30">
+    <cfRule type="expression" dxfId="29" priority="32">
       <formula>$D11&lt;&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="expression" dxfId="26" priority="28">
+    <cfRule type="expression" dxfId="28" priority="30">
       <formula>$E11=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="27">
+    <cfRule type="expression" dxfId="27" priority="29">
       <formula>$E11&lt;&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F11">
-    <cfRule type="expression" dxfId="24" priority="26">
+    <cfRule type="expression" dxfId="26" priority="28">
       <formula>$F11=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="25">
+    <cfRule type="expression" dxfId="25" priority="27">
       <formula>$F11&lt;&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G11">
-    <cfRule type="expression" dxfId="22" priority="24">
+    <cfRule type="expression" dxfId="24" priority="26">
       <formula>$G11=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="23">
+    <cfRule type="expression" dxfId="23" priority="25">
       <formula>$G11&lt;&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11">
-    <cfRule type="expression" dxfId="20" priority="21">
+    <cfRule type="expression" dxfId="22" priority="23">
       <formula>$H11&lt;&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="22">
+    <cfRule type="expression" dxfId="21" priority="24">
       <formula>$H11=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I11">
-    <cfRule type="expression" dxfId="18" priority="19">
+    <cfRule type="expression" dxfId="20" priority="21">
       <formula>$I11&lt;&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="20">
+    <cfRule type="expression" dxfId="19" priority="22">
       <formula>$I11=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11">
-    <cfRule type="expression" dxfId="16" priority="17">
+    <cfRule type="expression" dxfId="18" priority="19">
       <formula>$J11&lt;&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="18">
+    <cfRule type="expression" dxfId="17" priority="20">
       <formula>$J11=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11">
-    <cfRule type="expression" dxfId="14" priority="15">
+    <cfRule type="expression" dxfId="16" priority="17">
       <formula>$K11&lt;&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="16">
+    <cfRule type="expression" dxfId="15" priority="18">
       <formula>$K11=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L11">
-    <cfRule type="expression" dxfId="12" priority="13">
+    <cfRule type="expression" dxfId="14" priority="15">
       <formula>$L11&lt;&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="14">
+    <cfRule type="expression" dxfId="13" priority="16">
       <formula>$L11=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11">
-    <cfRule type="expression" dxfId="10" priority="12">
+    <cfRule type="expression" dxfId="12" priority="14">
       <formula>OR($C11&lt;&gt;0,$D11&lt;&gt;0,$E11&lt;&gt;0,$F11&lt;&gt;0,$G11&lt;&gt;0,$H11&lt;&gt;0,$I11&lt;&gt;0,$J11&lt;&gt;0,$K11&lt;&gt;0,$L11&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="expression" dxfId="9" priority="11">
+    <cfRule type="expression" dxfId="11" priority="13">
       <formula>OR($C11&lt;&gt;0,$D11&lt;&gt;0,$E11&lt;&gt;0,$F11&lt;&gt;0,$G11&lt;&gt;0,$H11&lt;&gt;0,$I11&lt;&gt;0,$J11&lt;&gt;0,$K11&lt;&gt;0,$L11&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="expression" dxfId="8" priority="9">
+    <cfRule type="expression" dxfId="10" priority="11">
       <formula>$B13&lt;30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N11">
-    <cfRule type="expression" dxfId="7" priority="7">
+    <cfRule type="expression" dxfId="9" priority="9">
       <formula>$N11&lt;&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="8">
+    <cfRule type="expression" dxfId="8" priority="10">
       <formula>$N11=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M11">
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="7" priority="8">
       <formula>$M11&lt;&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="6" priority="7">
       <formula>$N11=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O11">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>$O11&lt;&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>$O11=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P11">
+    <cfRule type="expression" dxfId="3" priority="3">
+      <formula>$P11=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="4">
+      <formula>$P11&lt;&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q11">
     <cfRule type="expression" dxfId="1" priority="1">
       <formula>$P11=0</formula>
     </cfRule>

</xml_diff>